<commit_message>
added bulk attendance excel and fixed the edit bug
</commit_message>
<xml_diff>
--- a/temp/bulkAttendanceTemplate.xlsx
+++ b/temp/bulkAttendanceTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aximos\HR_SOFTWARE\backend\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A893DABE-A09C-4A96-8F52-64CF50F7A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D3455-AF02-4DB3-8F0F-F2692FD54BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F42B38E-4008-4D45-BE84-50DEA61DBFA2}"/>
   </bookViews>
@@ -39,19 +39,19 @@
     <t>id</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>punchIn</t>
-  </si>
-  <si>
-    <t>punchOut</t>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>date (dd-MM-yyyy)</t>
+  </si>
+  <si>
+    <t>punchIn (HH:mm)</t>
+  </si>
+  <si>
+    <t>punchOut (HH:mm)</t>
   </si>
 </sst>
 </file>
@@ -406,10 +406,17 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>